<commit_message>
Updated the CalcExcessMortYLL class to feature updates made in its dependency - CalcExcessMortality
Signed-off-by: Mlad-en <mmladenov1992@gmail.com>
</commit_message>
<xml_diff>
--- a/data_output/Excess Mortality/Countries/2020/2020_AGE_AGGREGATED_TOTAL_EU_['Female', 'Male', 'Total']_(0-4) - (70-74).xlsx
+++ b/data_output/Excess Mortality/Countries/2020/2020_AGE_AGGREGATED_TOTAL_EU_['Female', 'Male', 'Total']_(0-4) - (70-74).xlsx
@@ -286,7 +286,7 @@
     <t>355.2 (±173.6)</t>
   </si>
   <si>
-    <t>1047.0 (±150.4)</t>
+    <t>1049.0 (±150.4)</t>
   </si>
   <si>
     <t>3357.6 (±193.1)</t>
@@ -298,7 +298,7 @@
     <t>46.4 (±25.1)</t>
   </si>
   <si>
-    <t>1421.0 (±185.2)</t>
+    <t>1420.0 (±185.2)</t>
   </si>
   <si>
     <t>-278.2 (±170.6)</t>
@@ -361,7 +361,7 @@
     <t>1958.4 (±172.1)</t>
   </si>
   <si>
-    <t>873.4 (±86.3)</t>
+    <t>877.4 (±86.3)</t>
   </si>
   <si>
     <t>140.6 (±32.5)</t>
@@ -379,7 +379,7 @@
     <t>4.7% (±2.4%)</t>
   </si>
   <si>
-    <t>9.8% (±1.6%)</t>
+    <t>9.8% (±1.5%)</t>
   </si>
   <si>
     <t>24.8% (±1.8%)</t>
@@ -454,7 +454,7 @@
     <t>14.9% (±1.5%)</t>
   </si>
   <si>
-    <t>12.2% (±1.3%)</t>
+    <t>12.3% (±1.4%)</t>
   </si>
   <si>
     <t>7.4% (±1.8%)</t>
@@ -472,7 +472,7 @@
     <t>8.9(±4.3)</t>
   </si>
   <si>
-    <t>20.1(±2.8)</t>
+    <t>20.1(±2.9)</t>
   </si>
   <si>
     <t>105.4(±6.1)</t>
@@ -484,7 +484,7 @@
     <t>11.1(±6.0)</t>
   </si>
   <si>
-    <t>29.1(±3.8)</t>
+    <t>29.0(±3.8)</t>
   </si>
   <si>
     <t>-10.6(±6.5)</t>
@@ -547,7 +547,7 @@
     <t>61.0(±5.4)</t>
   </si>
   <si>
-    <t>34.1(±3.3)</t>
+    <t>34.2(±3.4)</t>
   </si>
   <si>
     <t>15.2(±3.5)</t>
@@ -661,7 +661,7 @@
     <t>993.6 (±375.9)</t>
   </si>
   <si>
-    <t>2274.2 (±196.3)</t>
+    <t>2276.2 (±196.3)</t>
   </si>
   <si>
     <t>5771.4 (±343.6)</t>
@@ -736,7 +736,7 @@
     <t>4624.0 (±367.9)</t>
   </si>
   <si>
-    <t>1481.8 (±162.6)</t>
+    <t>1483.8 (±162.6)</t>
   </si>
   <si>
     <t>395.8 (±78.6)</t>
@@ -829,7 +829,7 @@
     <t>21.5% (±2.1%)</t>
   </si>
   <si>
-    <t>10.7% (±1.3%)</t>
+    <t>10.7% (±1.2%)</t>
   </si>
   <si>
     <t>10.3% (±2.2%)</t>
@@ -922,7 +922,7 @@
     <t>146.8(±11.7)</t>
   </si>
   <si>
-    <t>58.1(±6.4)</t>
+    <t>58.2(±6.4)</t>
   </si>
   <si>
     <t>40.4(±8.0)</t>
@@ -1036,7 +1036,7 @@
     <t>1348.8 (±536.8)</t>
   </si>
   <si>
-    <t>3321.2 (±234.5)</t>
+    <t>3325.2 (±234.5)</t>
   </si>
   <si>
     <t>9129.0 (±500.7)</t>
@@ -1048,7 +1048,7 @@
     <t>159.6 (±63.1)</t>
   </si>
   <si>
-    <t>4568.4 (±490.1)</t>
+    <t>4567.4 (±490.1)</t>
   </si>
   <si>
     <t>-672.0 (±304.5)</t>
@@ -1111,7 +1111,7 @@
     <t>6582.4 (±521.6)</t>
   </si>
   <si>
-    <t>2355.2 (±221.5)</t>
+    <t>2361.2 (±221.5)</t>
   </si>
   <si>
     <t>536.4 (±105.0)</t>
@@ -1204,7 +1204,7 @@
     <t>19.0% (±1.8%)</t>
   </si>
   <si>
-    <t>11.2% (±1.1%)</t>
+    <t>11.3% (±1.2%)</t>
   </si>
   <si>
     <t>9.4% (±2.0%)</t>
@@ -1297,7 +1297,7 @@
     <t>103.5(±8.2)</t>
   </si>
   <si>
-    <t>46.1(±4.3)</t>
+    <t>46.2(±4.3)</t>
   </si>
   <si>
     <t>28.2(±5.5)</t>
@@ -1907,7 +1907,7 @@
         <v>10600</v>
       </c>
       <c r="H3">
-        <v>11770</v>
+        <v>11772</v>
       </c>
       <c r="I3">
         <v>10723</v>
@@ -1928,7 +1928,7 @@
         <v>10873.4</v>
       </c>
       <c r="O3">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="P3">
         <v>150.4</v>
@@ -1937,7 +1937,7 @@
         <v>9.800000000000001</v>
       </c>
       <c r="R3">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="S3" t="s">
         <v>58</v>
@@ -1955,7 +1955,7 @@
         <v>20.1</v>
       </c>
       <c r="X3">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="Y3" t="s">
         <v>151</v>
@@ -2215,7 +2215,7 @@
         <v>12902</v>
       </c>
       <c r="H7">
-        <v>14825</v>
+        <v>14824</v>
       </c>
       <c r="I7">
         <v>13404</v>
@@ -2236,7 +2236,7 @@
         <v>13589.2</v>
       </c>
       <c r="O7">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="P7">
         <v>185.2</v>
@@ -2260,7 +2260,7 @@
         <v>4888989</v>
       </c>
       <c r="W7">
-        <v>29.1</v>
+        <v>29</v>
       </c>
       <c r="X7">
         <v>3.8</v>
@@ -3832,7 +3832,7 @@
         <v>6876</v>
       </c>
       <c r="H28">
-        <v>8017</v>
+        <v>8021</v>
       </c>
       <c r="I28">
         <v>7143.599999999996</v>
@@ -3853,16 +3853,16 @@
         <v>7229.899999999996</v>
       </c>
       <c r="O28">
-        <v>873.4</v>
+        <v>877.4</v>
       </c>
       <c r="P28">
         <v>86.3</v>
       </c>
       <c r="Q28">
-        <v>12.2</v>
+        <v>12.3</v>
       </c>
       <c r="R28">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="S28" t="s">
         <v>83</v>
@@ -3877,10 +3877,10 @@
         <v>2564041</v>
       </c>
       <c r="W28">
-        <v>34.1</v>
+        <v>34.2</v>
       </c>
       <c r="X28">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="Y28" t="s">
         <v>176</v>
@@ -4384,7 +4384,7 @@
         <v>16911</v>
       </c>
       <c r="H3">
-        <v>19859</v>
+        <v>19861</v>
       </c>
       <c r="I3">
         <v>17584.8</v>
@@ -4405,7 +4405,7 @@
         <v>17781.1</v>
       </c>
       <c r="O3">
-        <v>2274.2</v>
+        <v>2276.2</v>
       </c>
       <c r="P3">
         <v>196.3</v>
@@ -6309,7 +6309,7 @@
         <v>13540</v>
       </c>
       <c r="H28">
-        <v>15286</v>
+        <v>15288</v>
       </c>
       <c r="I28">
         <v>13804.2</v>
@@ -6330,7 +6330,7 @@
         <v>13966.8</v>
       </c>
       <c r="O28">
-        <v>1481.8</v>
+        <v>1483.8</v>
       </c>
       <c r="P28">
         <v>162.6</v>
@@ -6339,7 +6339,7 @@
         <v>10.7</v>
       </c>
       <c r="R28">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="S28" t="s">
         <v>208</v>
@@ -6354,7 +6354,7 @@
         <v>2549303</v>
       </c>
       <c r="W28">
-        <v>58.1</v>
+        <v>58.2</v>
       </c>
       <c r="X28">
         <v>6.4</v>
@@ -6861,7 +6861,7 @@
         <v>27511</v>
       </c>
       <c r="H3">
-        <v>31629</v>
+        <v>31633</v>
       </c>
       <c r="I3">
         <v>28307.79999999999</v>
@@ -6882,7 +6882,7 @@
         <v>28542.29999999999</v>
       </c>
       <c r="O3">
-        <v>3321.2</v>
+        <v>3325.2</v>
       </c>
       <c r="P3">
         <v>234.5</v>
@@ -7169,7 +7169,7 @@
         <v>36850</v>
       </c>
       <c r="H7">
-        <v>42720</v>
+        <v>42719</v>
       </c>
       <c r="I7">
         <v>38151.60000000001</v>
@@ -7190,7 +7190,7 @@
         <v>38641.7</v>
       </c>
       <c r="O7">
-        <v>4568.4</v>
+        <v>4567.4</v>
       </c>
       <c r="P7">
         <v>490.1</v>
@@ -8786,7 +8786,7 @@
         <v>20416</v>
       </c>
       <c r="H28">
-        <v>23303</v>
+        <v>23309</v>
       </c>
       <c r="I28">
         <v>20947.8</v>
@@ -8807,16 +8807,16 @@
         <v>21169.3</v>
       </c>
       <c r="O28">
-        <v>2355.2</v>
+        <v>2361.2</v>
       </c>
       <c r="P28">
         <v>221.5</v>
       </c>
       <c r="Q28">
-        <v>11.2</v>
+        <v>11.3</v>
       </c>
       <c r="R28">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="S28" t="s">
         <v>333</v>
@@ -8831,7 +8831,7 @@
         <v>5113344</v>
       </c>
       <c r="W28">
-        <v>46.1</v>
+        <v>46.2</v>
       </c>
       <c r="X28">
         <v>4.3</v>

</xml_diff>

<commit_message>
Adding pytest to the project. Adding a new branch to refactor project.
Signed-off-by: Mlad-en <mmladenov1992@gmail.com>
</commit_message>
<xml_diff>
--- a/data_output/Excess Mortality/Countries/2020/2020_AGE_AGGREGATED_TOTAL_EU_['Female', 'Male', 'Total']_(0-4) - (70-74).xlsx
+++ b/data_output/Excess Mortality/Countries/2020/2020_AGE_AGGREGATED_TOTAL_EU_['Female', 'Male', 'Total']_(0-4) - (70-74).xlsx
@@ -250,10 +250,10 @@
     <t>864.0 (±32.6)</t>
   </si>
   <si>
-    <t>16771.4 (±128.5)</t>
-  </si>
-  <si>
-    <t>4136.0 (±27.3)</t>
+    <t>16761.8 (±126.9)</t>
+  </si>
+  <si>
+    <t>4136.2 (±27.4)</t>
   </si>
   <si>
     <t>50492.8 (±1174.3)</t>
@@ -286,10 +286,10 @@
     <t>355.2 (±173.6)</t>
   </si>
   <si>
-    <t>1049.0 (±150.4)</t>
-  </si>
-  <si>
-    <t>3357.6 (±193.1)</t>
+    <t>998.0 (±150.4)</t>
+  </si>
+  <si>
+    <t>3361.6 (±193.1)</t>
   </si>
   <si>
     <t>536.8 (±174.7)</t>
@@ -298,19 +298,19 @@
     <t>46.4 (±25.1)</t>
   </si>
   <si>
-    <t>1420.0 (±185.2)</t>
+    <t>1419.0 (±185.2)</t>
   </si>
   <si>
     <t>-278.2 (±170.6)</t>
   </si>
   <si>
-    <t>146.8 (±46.1)</t>
+    <t>148.8 (±46.1)</t>
   </si>
   <si>
     <t>202.2 (±60.0)</t>
   </si>
   <si>
-    <t>4808.0 (±749.6)</t>
+    <t>4815.0 (±749.6)</t>
   </si>
   <si>
     <t>866.4 (±102.0)</t>
@@ -322,10 +322,10 @@
     <t>12.0 (±14.6)</t>
   </si>
   <si>
-    <t>5418.0 (±1069.6)</t>
-  </si>
-  <si>
-    <t>-119.8 (±134.4)</t>
+    <t>5429.0 (±1069.6)</t>
+  </si>
+  <si>
+    <t>-85.8 (±134.4)</t>
   </si>
   <si>
     <t>-1.8 (±3.3)</t>
@@ -337,16 +337,16 @@
     <t>27.4 (±17.4)</t>
   </si>
   <si>
-    <t>13.8 (±13.0)</t>
-  </si>
-  <si>
-    <t>146.0 (±32.6)</t>
-  </si>
-  <si>
-    <t>1015.6 (±128.5)</t>
-  </si>
-  <si>
-    <t>-45.0 (±27.3)</t>
+    <t>15.8 (±13.0)</t>
+  </si>
+  <si>
+    <t>136.0 (±32.6)</t>
+  </si>
+  <si>
+    <t>1029.2 (±126.9)</t>
+  </si>
+  <si>
+    <t>-41.2 (±27.4)</t>
   </si>
   <si>
     <t>11159.2 (±1174.3)</t>
@@ -355,7 +355,7 @@
     <t>780.4 (±91.2)</t>
   </si>
   <si>
-    <t>6537.0 (±440.4)</t>
+    <t>6554.0 (±440.4)</t>
   </si>
   <si>
     <t>1958.4 (±172.1)</t>
@@ -364,10 +364,10 @@
     <t>877.4 (±86.3)</t>
   </si>
   <si>
-    <t>140.6 (±32.5)</t>
-  </si>
-  <si>
-    <t>6108.2 (±277.0)</t>
+    <t>144.6 (±32.5)</t>
+  </si>
+  <si>
+    <t>5410.2 (±277.0)</t>
   </si>
   <si>
     <t>-234.0 (±197.7)</t>
@@ -379,10 +379,10 @@
     <t>4.7% (±2.4%)</t>
   </si>
   <si>
-    <t>9.8% (±1.5%)</t>
-  </si>
-  <si>
-    <t>24.8% (±1.8%)</t>
+    <t>9.3% (±1.5%)</t>
+  </si>
+  <si>
+    <t>24.8% (±1.7%)</t>
   </si>
   <si>
     <t>10.2% (±3.5%)</t>
@@ -397,7 +397,7 @@
     <t>-4.4% (±2.5%)</t>
   </si>
   <si>
-    <t>9.2% (±3.1%)</t>
+    <t>9.3% (±3.1%)</t>
   </si>
   <si>
     <t>3.9% (±1.2%)</t>
@@ -418,7 +418,7 @@
     <t>11.1% (±2.4%)</t>
   </si>
   <si>
-    <t>-3.5% (±3.6%)</t>
+    <t>-2.5% (±3.6%)</t>
   </si>
   <si>
     <t>-6.0% (±9.4%)</t>
@@ -430,16 +430,16 @@
     <t>6.5% (±4.2%)</t>
   </si>
   <si>
-    <t>3.4% (±3.2%)</t>
-  </si>
-  <si>
-    <t>16.9% (±4.3%)</t>
-  </si>
-  <si>
-    <t>6.1% (±0.9%)</t>
-  </si>
-  <si>
-    <t>-1.1% (±0.6%)</t>
+    <t>3.9% (±3.2%)</t>
+  </si>
+  <si>
+    <t>15.7% (±4.2%)</t>
+  </si>
+  <si>
+    <t>6.1% (±0.8%)</t>
+  </si>
+  <si>
+    <t>-1.0% (±0.6%)</t>
   </si>
   <si>
     <t>22.1% (±2.8%)</t>
@@ -457,10 +457,10 @@
     <t>12.3% (±1.4%)</t>
   </si>
   <si>
-    <t>7.4% (±1.8%)</t>
-  </si>
-  <si>
-    <t>19.6% (±1.0%)</t>
+    <t>7.6% (±1.8%)</t>
+  </si>
+  <si>
+    <t>17.4% (±1.0%)</t>
   </si>
   <si>
     <t>-2.8% (±2.3%)</t>
@@ -472,10 +472,10 @@
     <t>8.9(±4.3)</t>
   </si>
   <si>
-    <t>20.1(±2.9)</t>
-  </si>
-  <si>
-    <t>105.4(±6.1)</t>
+    <t>19.1(±2.9)</t>
+  </si>
+  <si>
+    <t>105.5(±6.1)</t>
   </si>
   <si>
     <t>29.2(±9.5)</t>
@@ -490,7 +490,7 @@
     <t>-10.6(±6.5)</t>
   </si>
   <si>
-    <t>24.1(±7.5)</t>
+    <t>24.4(±7.5)</t>
   </si>
   <si>
     <t>8.2(±2.4)</t>
@@ -511,7 +511,7 @@
     <t>20.6(±4.0)</t>
   </si>
   <si>
-    <t>-13.5(±15.1)</t>
+    <t>-9.7(±15.2)</t>
   </si>
   <si>
     <t>-10.1(±18.5)</t>
@@ -523,16 +523,16 @@
     <t>9.6(±6.0)</t>
   </si>
   <si>
-    <t>6.1(±5.7)</t>
-  </si>
-  <si>
-    <t>50.0(±11.1)</t>
-  </si>
-  <si>
-    <t>12.8(±1.6)</t>
-  </si>
-  <si>
-    <t>-1.9(±1.2)</t>
+    <t>7.0(±5.7)</t>
+  </si>
+  <si>
+    <t>46.6(±11.1)</t>
+  </si>
+  <si>
+    <t>13.0(±1.6)</t>
+  </si>
+  <si>
+    <t>-1.7(±1.1)</t>
   </si>
   <si>
     <t>62.7(±6.6)</t>
@@ -541,7 +541,7 @@
     <t>16.4(±1.9)</t>
   </si>
   <si>
-    <t>73.7(±4.9)</t>
+    <t>73.9(±4.9)</t>
   </si>
   <si>
     <t>61.0(±5.4)</t>
@@ -550,10 +550,10 @@
     <t>34.2(±3.4)</t>
   </si>
   <si>
-    <t>15.2(±3.5)</t>
-  </si>
-  <si>
-    <t>28.6(±1.3)</t>
+    <t>15.7(±3.5)</t>
+  </si>
+  <si>
+    <t>25.3(±1.3)</t>
   </si>
   <si>
     <t>-5.1(±4.3)</t>
@@ -625,10 +625,10 @@
     <t>1471.6 (±40.4)</t>
   </si>
   <si>
-    <t>23607.2 (±225.4)</t>
-  </si>
-  <si>
-    <t>6324.4 (±60.3)</t>
+    <t>23577.6 (±236.8)</t>
+  </si>
+  <si>
+    <t>6325.0 (±60.0)</t>
   </si>
   <si>
     <t>102191.6 (±1501.6)</t>
@@ -661,10 +661,10 @@
     <t>993.6 (±375.9)</t>
   </si>
   <si>
-    <t>2276.2 (±196.3)</t>
-  </si>
-  <si>
-    <t>5771.4 (±343.6)</t>
+    <t>2079.2 (±196.3)</t>
+  </si>
+  <si>
+    <t>5772.4 (±343.6)</t>
   </si>
   <si>
     <t>1135.8 (±240.3)</t>
@@ -673,19 +673,19 @@
     <t>113.2 (±39.3)</t>
   </si>
   <si>
-    <t>3147.4 (±309.9)</t>
+    <t>3153.4 (±309.9)</t>
   </si>
   <si>
     <t>-393.8 (±144.0)</t>
   </si>
   <si>
-    <t>165.4 (±74.6)</t>
+    <t>169.4 (±74.6)</t>
   </si>
   <si>
     <t>260.0 (±103.0)</t>
   </si>
   <si>
-    <t>8038.4 (±528.2)</t>
+    <t>8065.4 (±528.2)</t>
   </si>
   <si>
     <t>1130.4 (±246.4)</t>
@@ -697,10 +697,10 @@
     <t>11.0 (±14.6)</t>
   </si>
   <si>
-    <t>14210.2 (±2155.3)</t>
-  </si>
-  <si>
-    <t>-178.0 (±229.9)</t>
+    <t>14254.2 (±2155.3)</t>
+  </si>
+  <si>
+    <t>-28.0 (±229.9)</t>
   </si>
   <si>
     <t>-0.8 (±3.9)</t>
@@ -712,16 +712,16 @@
     <t>84.8 (±29.5)</t>
   </si>
   <si>
-    <t>72.6 (±24.2)</t>
-  </si>
-  <si>
-    <t>317.4 (±40.4)</t>
-  </si>
-  <si>
-    <t>2192.8 (±225.4)</t>
-  </si>
-  <si>
-    <t>-107.4 (±60.3)</t>
+    <t>73.6 (±24.2)</t>
+  </si>
+  <si>
+    <t>290.4 (±40.4)</t>
+  </si>
+  <si>
+    <t>2263.4 (±236.8)</t>
+  </si>
+  <si>
+    <t>-107.0 (±60.0)</t>
   </si>
   <si>
     <t>22280.4 (±1501.6)</t>
@@ -730,19 +730,19 @@
     <t>1663.8 (±128.1)</t>
   </si>
   <si>
-    <t>13095.0 (±728.7)</t>
+    <t>13133.0 (±728.7)</t>
   </si>
   <si>
     <t>4624.0 (±367.9)</t>
   </si>
   <si>
-    <t>1483.8 (±162.6)</t>
-  </si>
-  <si>
-    <t>395.8 (±78.6)</t>
-  </si>
-  <si>
-    <t>10183.0 (±430.0)</t>
+    <t>1485.8 (±162.6)</t>
+  </si>
+  <si>
+    <t>410.8 (±78.6)</t>
+  </si>
+  <si>
+    <t>9703.0 (±430.0)</t>
   </si>
   <si>
     <t>99.0 (±541.5)</t>
@@ -754,7 +754,7 @@
     <t>7.7% (±3.0%)</t>
   </si>
   <si>
-    <t>12.9% (±1.2%)</t>
+    <t>11.8% (±1.2%)</t>
   </si>
   <si>
     <t>22.9% (±1.7%)</t>
@@ -772,13 +772,13 @@
     <t>-4.1% (±1.4%)</t>
   </si>
   <si>
-    <t>5.0% (±2.3%)</t>
+    <t>5.1% (±2.3%)</t>
   </si>
   <si>
     <t>2.7% (±1.1%)</t>
   </si>
   <si>
-    <t>7.9% (±0.6%)</t>
+    <t>7.9% (±0.5%)</t>
   </si>
   <si>
     <t>6.2% (±1.4%)</t>
@@ -790,10 +790,10 @@
     <t>2.9% (±3.8%)</t>
   </si>
   <si>
-    <t>17.5% (±3.0%)</t>
-  </si>
-  <si>
-    <t>-2.7% (±3.3%)</t>
+    <t>17.6% (±3.1%)</t>
+  </si>
+  <si>
+    <t>-0.4% (±3.4%)</t>
   </si>
   <si>
     <t>-1.5% (±6.9%)</t>
@@ -805,13 +805,13 @@
     <t>11.2% (±4.2%)</t>
   </si>
   <si>
-    <t>11.1% (±4.0%)</t>
-  </si>
-  <si>
-    <t>21.6% (±3.3%)</t>
-  </si>
-  <si>
-    <t>9.3% (±1.0%)</t>
+    <t>11.3% (±4.0%)</t>
+  </si>
+  <si>
+    <t>19.7% (±3.2%)</t>
+  </si>
+  <si>
+    <t>9.6% (±1.1%)</t>
   </si>
   <si>
     <t>-1.7% (±0.9%)</t>
@@ -829,13 +829,13 @@
     <t>21.5% (±2.1%)</t>
   </si>
   <si>
-    <t>10.7% (±1.2%)</t>
-  </si>
-  <si>
-    <t>10.3% (±2.2%)</t>
-  </si>
-  <si>
-    <t>16.2% (±0.8%)</t>
+    <t>10.8% (±1.3%)</t>
+  </si>
+  <si>
+    <t>10.7% (±2.2%)</t>
+  </si>
+  <si>
+    <t>15.4% (±0.8%)</t>
   </si>
   <si>
     <t>0.8% (±4.3%)</t>
@@ -847,10 +847,10 @@
     <t>24.6(±9.3)</t>
   </si>
   <si>
-    <t>43.2(±3.7)</t>
-  </si>
-  <si>
-    <t>183.6(±10.9)</t>
+    <t>39.5(±3.7)</t>
+  </si>
+  <si>
+    <t>183.6(±11.0)</t>
   </si>
   <si>
     <t>61.9(±13.1)</t>
@@ -859,19 +859,19 @@
     <t>27.8(±9.6)</t>
   </si>
   <si>
-    <t>63.5(±6.3)</t>
+    <t>63.6(±6.3)</t>
   </si>
   <si>
     <t>-14.7(±5.4)</t>
   </si>
   <si>
-    <t>27.9(±12.6)</t>
+    <t>28.6(±12.6)</t>
   </si>
   <si>
     <t>10.3(±4.1)</t>
   </si>
   <si>
-    <t>26.7(±1.8)</t>
+    <t>26.8(±1.8)</t>
   </si>
   <si>
     <t>24.0(±5.3)</t>
@@ -883,10 +883,10 @@
     <t>6.2(±8.3)</t>
   </si>
   <si>
-    <t>54.2(±8.2)</t>
-  </si>
-  <si>
-    <t>-21.5(±27.8)</t>
+    <t>54.4(±8.2)</t>
+  </si>
+  <si>
+    <t>-3.4(±27.8)</t>
   </si>
   <si>
     <t>-4.5(±21.8)</t>
@@ -898,13 +898,13 @@
     <t>28.4(±9.9)</t>
   </si>
   <si>
-    <t>29.1(±9.6)</t>
-  </si>
-  <si>
-    <t>108.4(±13.8)</t>
-  </si>
-  <si>
-    <t>27.3(±2.8)</t>
+    <t>29.5(±9.6)</t>
+  </si>
+  <si>
+    <t>99.2(±13.8)</t>
+  </si>
+  <si>
+    <t>28.2(±2.9)</t>
   </si>
   <si>
     <t>-4.2(±2.3)</t>
@@ -916,19 +916,19 @@
     <t>37.5(±2.9)</t>
   </si>
   <si>
-    <t>147.3(±8.2)</t>
+    <t>147.7(±8.2)</t>
   </si>
   <si>
     <t>146.8(±11.7)</t>
   </si>
   <si>
-    <t>58.2(±6.4)</t>
-  </si>
-  <si>
-    <t>40.4(±8.0)</t>
-  </si>
-  <si>
-    <t>47.7(±2.0)</t>
+    <t>58.3(±6.4)</t>
+  </si>
+  <si>
+    <t>42.0(±8.0)</t>
+  </si>
+  <si>
+    <t>45.4(±2.0)</t>
   </si>
   <si>
     <t>2.1(±11.3)</t>
@@ -1000,10 +1000,10 @@
     <t>2335.6 (±47.9)</t>
   </si>
   <si>
-    <t>40378.6 (±326.0)</t>
-  </si>
-  <si>
-    <t>10460.4 (±56.3)</t>
+    <t>40339.4 (±336.3)</t>
+  </si>
+  <si>
+    <t>10461.2 (±55.7)</t>
   </si>
   <si>
     <t>152684.4 (±2638.3)</t>
@@ -1036,10 +1036,10 @@
     <t>1348.8 (±536.8)</t>
   </si>
   <si>
-    <t>3325.2 (±234.5)</t>
-  </si>
-  <si>
-    <t>9129.0 (±500.7)</t>
+    <t>3077.2 (±234.5)</t>
+  </si>
+  <si>
+    <t>9134.0 (±500.7)</t>
   </si>
   <si>
     <t>1672.6 (±393.0)</t>
@@ -1048,19 +1048,19 @@
     <t>159.6 (±63.1)</t>
   </si>
   <si>
-    <t>4567.4 (±490.1)</t>
+    <t>4572.4 (±490.1)</t>
   </si>
   <si>
     <t>-672.0 (±304.5)</t>
   </si>
   <si>
-    <t>312.2 (±117.1)</t>
+    <t>318.2 (±117.1)</t>
   </si>
   <si>
     <t>462.2 (±92.2)</t>
   </si>
   <si>
-    <t>12846.4 (±619.4)</t>
+    <t>12880.4 (±619.4)</t>
   </si>
   <si>
     <t>1996.8 (±248.3)</t>
@@ -1072,10 +1072,10 @@
     <t>23.0 (±13.6)</t>
   </si>
   <si>
-    <t>19628.2 (±3215.8)</t>
-  </si>
-  <si>
-    <t>-297.8 (±356.6)</t>
+    <t>19683.2 (±3215.8)</t>
+  </si>
+  <si>
+    <t>-113.8 (±356.6)</t>
   </si>
   <si>
     <t>-2.6 (±6.2)</t>
@@ -1087,16 +1087,16 @@
     <t>112.2 (±45.2)</t>
   </si>
   <si>
-    <t>86.4 (±33.0)</t>
-  </si>
-  <si>
-    <t>463.4 (±47.9)</t>
-  </si>
-  <si>
-    <t>3208.4 (±326.0)</t>
-  </si>
-  <si>
-    <t>-152.4 (±56.3)</t>
+    <t>89.4 (±33.0)</t>
+  </si>
+  <si>
+    <t>426.4 (±47.9)</t>
+  </si>
+  <si>
+    <t>3292.6 (±336.3)</t>
+  </si>
+  <si>
+    <t>-148.2 (±55.7)</t>
   </si>
   <si>
     <t>33439.6 (±2638.3)</t>
@@ -1105,19 +1105,19 @@
     <t>2444.2 (±172.2)</t>
   </si>
   <si>
-    <t>19632.0 (±937.5)</t>
+    <t>19687.0 (±937.5)</t>
   </si>
   <si>
     <t>6582.4 (±521.6)</t>
   </si>
   <si>
-    <t>2361.2 (±221.5)</t>
-  </si>
-  <si>
-    <t>536.4 (±105.0)</t>
-  </si>
-  <si>
-    <t>16315.2 (±439.1)</t>
+    <t>2363.2 (±221.5)</t>
+  </si>
+  <si>
+    <t>555.4 (±105.0)</t>
+  </si>
+  <si>
+    <t>15113.2 (±439.1)</t>
   </si>
   <si>
     <t>-135.0 (±732.7)</t>
@@ -1129,7 +1129,7 @@
     <t>6.6% (±2.7%)</t>
   </si>
   <si>
-    <t>11.7% (±0.9%)</t>
+    <t>10.9% (±0.9%)</t>
   </si>
   <si>
     <t>23.5% (±1.5%)</t>
@@ -1147,13 +1147,13 @@
     <t>-4.2% (±1.8%)</t>
   </si>
   <si>
-    <t>6.3% (±2.4%)</t>
+    <t>6.4% (±2.4%)</t>
   </si>
   <si>
     <t>3.1% (±0.6%)</t>
   </si>
   <si>
-    <t>8.3% (±0.5%)</t>
+    <t>8.3% (±0.4%)</t>
   </si>
   <si>
     <t>7.3% (±1.0%)</t>
@@ -1165,10 +1165,10 @@
     <t>3.7% (±2.2%)</t>
   </si>
   <si>
-    <t>15.1% (±2.8%)</t>
-  </si>
-  <si>
-    <t>-3.0% (±3.3%)</t>
+    <t>15.1% (±2.7%)</t>
+  </si>
+  <si>
+    <t>-1.1% (±3.4%)</t>
   </si>
   <si>
     <t>-3.2% (±6.8%)</t>
@@ -1180,16 +1180,16 @@
     <t>9.5% (±4.0%)</t>
   </si>
   <si>
-    <t>8.2% (±3.3%)</t>
-  </si>
-  <si>
-    <t>19.8% (±2.4%)</t>
-  </si>
-  <si>
-    <t>7.9% (±0.8%)</t>
-  </si>
-  <si>
-    <t>-1.5% (±0.5%)</t>
+    <t>8.5% (±3.3%)</t>
+  </si>
+  <si>
+    <t>18.3% (±2.4%)</t>
+  </si>
+  <si>
+    <t>8.2% (±0.9%)</t>
+  </si>
+  <si>
+    <t>-1.4% (±0.5%)</t>
   </si>
   <si>
     <t>21.9% (±2.1%)</t>
@@ -1198,7 +1198,7 @@
     <t>9.2% (±0.7%)</t>
   </si>
   <si>
-    <t>20.7% (±1.2%)</t>
+    <t>20.8% (±1.2%)</t>
   </si>
   <si>
     <t>19.0% (±1.8%)</t>
@@ -1207,10 +1207,10 @@
     <t>11.3% (±1.2%)</t>
   </si>
   <si>
-    <t>9.4% (±2.0%)</t>
-  </si>
-  <si>
-    <t>17.3% (±0.5%)</t>
+    <t>9.7% (±2.0%)</t>
+  </si>
+  <si>
+    <t>16.1% (±0.6%)</t>
   </si>
   <si>
     <t>-0.7% (±3.4%)</t>
@@ -1222,10 +1222,10 @@
     <t>16.8(±6.6)</t>
   </si>
   <si>
-    <t>31.7(±2.2)</t>
-  </si>
-  <si>
-    <t>144.2(±7.9)</t>
+    <t>29.3(±2.3)</t>
+  </si>
+  <si>
+    <t>144.3(±7.9)</t>
   </si>
   <si>
     <t>45.5(±10.7)</t>
@@ -1240,7 +1240,7 @@
     <t>-12.7(±5.8)</t>
   </si>
   <si>
-    <t>26.0(±9.7)</t>
+    <t>26.5(±9.7)</t>
   </si>
   <si>
     <t>9.2(±1.9)</t>
@@ -1258,10 +1258,10 @@
     <t>6.7(±4.0)</t>
   </si>
   <si>
-    <t>37.3(±6.1)</t>
-  </si>
-  <si>
-    <t>-17.3(±20.7)</t>
+    <t>37.4(±6.2)</t>
+  </si>
+  <si>
+    <t>-6.6(±20.7)</t>
   </si>
   <si>
     <t>-7.3(±17.4)</t>
@@ -1273,16 +1273,16 @@
     <t>19.2(±7.7)</t>
   </si>
   <si>
-    <t>18.1(±7.0)</t>
-  </si>
-  <si>
-    <t>79.2(±8.2)</t>
-  </si>
-  <si>
-    <t>20.1(±2.1)</t>
-  </si>
-  <si>
-    <t>-3.1(±1.2)</t>
+    <t>18.8(±6.9)</t>
+  </si>
+  <si>
+    <t>72.9(±8.2)</t>
+  </si>
+  <si>
+    <t>20.6(±2.1)</t>
+  </si>
+  <si>
+    <t>-3.0(±1.1)</t>
   </si>
   <si>
     <t>94.9(±7.5)</t>
@@ -1291,7 +1291,7 @@
     <t>26.6(±1.9)</t>
   </si>
   <si>
-    <t>110.5(±5.3)</t>
+    <t>110.8(±5.3)</t>
   </si>
   <si>
     <t>103.5(±8.2)</t>
@@ -1300,10 +1300,10 @@
     <t>46.2(±4.3)</t>
   </si>
   <si>
-    <t>28.2(±5.5)</t>
-  </si>
-  <si>
-    <t>38.2(±1.0)</t>
+    <t>29.2(±5.5)</t>
+  </si>
+  <si>
+    <t>35.4(±1.0)</t>
   </si>
   <si>
     <t>-1.4(±7.8)</t>
@@ -1907,7 +1907,7 @@
         <v>10600</v>
       </c>
       <c r="H3">
-        <v>11772</v>
+        <v>11721</v>
       </c>
       <c r="I3">
         <v>10723</v>
@@ -1928,13 +1928,13 @@
         <v>10873.4</v>
       </c>
       <c r="O3">
-        <v>1049</v>
+        <v>998</v>
       </c>
       <c r="P3">
         <v>150.4</v>
       </c>
       <c r="Q3">
-        <v>9.800000000000001</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="R3">
         <v>1.5</v>
@@ -1952,7 +1952,7 @@
         <v>5220663</v>
       </c>
       <c r="W3">
-        <v>20.1</v>
+        <v>19.1</v>
       </c>
       <c r="X3">
         <v>2.9</v>
@@ -1984,7 +1984,7 @@
         <v>12957</v>
       </c>
       <c r="H4">
-        <v>16903</v>
+        <v>16907</v>
       </c>
       <c r="I4">
         <v>13545.4</v>
@@ -2005,7 +2005,7 @@
         <v>13738.5</v>
       </c>
       <c r="O4">
-        <v>3357.6</v>
+        <v>3361.6</v>
       </c>
       <c r="P4">
         <v>193.1</v>
@@ -2014,7 +2014,7 @@
         <v>24.8</v>
       </c>
       <c r="R4">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="S4" t="s">
         <v>59</v>
@@ -2029,7 +2029,7 @@
         <v>3185698</v>
       </c>
       <c r="W4">
-        <v>105.4</v>
+        <v>105.5</v>
       </c>
       <c r="X4">
         <v>6.1</v>
@@ -2215,7 +2215,7 @@
         <v>12902</v>
       </c>
       <c r="H7">
-        <v>14824</v>
+        <v>14823</v>
       </c>
       <c r="I7">
         <v>13404</v>
@@ -2236,7 +2236,7 @@
         <v>13589.2</v>
       </c>
       <c r="O7">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="P7">
         <v>185.2</v>
@@ -2369,7 +2369,7 @@
         <v>1507</v>
       </c>
       <c r="H9">
-        <v>1745</v>
+        <v>1747</v>
       </c>
       <c r="I9">
         <v>1598.2</v>
@@ -2390,13 +2390,13 @@
         <v>1644.299999999999</v>
       </c>
       <c r="O9">
-        <v>146.8</v>
+        <v>148.8</v>
       </c>
       <c r="P9">
         <v>46.1</v>
       </c>
       <c r="Q9">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="R9">
         <v>3.1</v>
@@ -2414,7 +2414,7 @@
         <v>610017</v>
       </c>
       <c r="W9">
-        <v>24.1</v>
+        <v>24.4</v>
       </c>
       <c r="X9">
         <v>7.5</v>
@@ -2523,7 +2523,7 @@
         <v>53445</v>
       </c>
       <c r="H11">
-        <v>58325</v>
+        <v>58332</v>
       </c>
       <c r="I11">
         <v>53517.00000000001</v>
@@ -2544,7 +2544,7 @@
         <v>54266.60000000001</v>
       </c>
       <c r="O11">
-        <v>4808</v>
+        <v>4815</v>
       </c>
       <c r="P11">
         <v>749.6</v>
@@ -2831,7 +2831,7 @@
         <v>46670</v>
       </c>
       <c r="H15">
-        <v>54382</v>
+        <v>54393</v>
       </c>
       <c r="I15">
         <v>48964</v>
@@ -2852,7 +2852,7 @@
         <v>50033.6</v>
       </c>
       <c r="O15">
-        <v>5418</v>
+        <v>5429</v>
       </c>
       <c r="P15">
         <v>1069.6</v>
@@ -2908,7 +2908,7 @@
         <v>3143</v>
       </c>
       <c r="H16">
-        <v>3327</v>
+        <v>3361</v>
       </c>
       <c r="I16">
         <v>3446.8</v>
@@ -2929,13 +2929,13 @@
         <v>3581.2</v>
       </c>
       <c r="O16">
-        <v>-119.8</v>
+        <v>-85.8</v>
       </c>
       <c r="P16">
         <v>134.4</v>
       </c>
       <c r="Q16">
-        <v>-3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="R16">
         <v>3.6</v>
@@ -2953,10 +2953,10 @@
         <v>888614</v>
       </c>
       <c r="W16">
-        <v>-13.5</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="X16">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="Y16" t="s">
         <v>164</v>
@@ -3216,7 +3216,7 @@
         <v>387</v>
       </c>
       <c r="H20">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="I20">
         <v>404.2</v>
@@ -3237,13 +3237,13 @@
         <v>417.2</v>
       </c>
       <c r="O20">
-        <v>13.8</v>
+        <v>15.8</v>
       </c>
       <c r="P20">
         <v>13</v>
       </c>
       <c r="Q20">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="R20">
         <v>3.2</v>
@@ -3261,7 +3261,7 @@
         <v>226417</v>
       </c>
       <c r="W20">
-        <v>6.1</v>
+        <v>7</v>
       </c>
       <c r="X20">
         <v>5.7</v>
@@ -3293,7 +3293,7 @@
         <v>813</v>
       </c>
       <c r="H21">
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="I21">
         <v>863.9999999999997</v>
@@ -3314,16 +3314,16 @@
         <v>896.5999999999997</v>
       </c>
       <c r="O21">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="P21">
         <v>32.6</v>
       </c>
       <c r="Q21">
-        <v>16.9</v>
+        <v>15.7</v>
       </c>
       <c r="R21">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="S21" t="s">
         <v>76</v>
@@ -3338,7 +3338,7 @@
         <v>292082</v>
       </c>
       <c r="W21">
-        <v>50</v>
+        <v>46.6</v>
       </c>
       <c r="X21">
         <v>11.1</v>
@@ -3355,52 +3355,52 @@
         <v>46</v>
       </c>
       <c r="C22">
-        <v>16613</v>
+        <v>16614</v>
       </c>
       <c r="D22">
-        <v>16495</v>
+        <v>16470</v>
       </c>
       <c r="E22">
-        <v>16181</v>
+        <v>16178</v>
       </c>
       <c r="F22">
-        <v>16530</v>
+        <v>16511</v>
       </c>
       <c r="G22">
-        <v>16442</v>
+        <v>16440</v>
       </c>
       <c r="H22">
-        <v>17787</v>
+        <v>17791</v>
       </c>
       <c r="I22">
-        <v>16771.4</v>
+        <v>16761.8</v>
       </c>
       <c r="J22">
-        <v>146.6</v>
+        <v>144.8</v>
       </c>
       <c r="K22">
         <v>1.96</v>
       </c>
       <c r="L22">
-        <v>128.5</v>
+        <v>126.9</v>
       </c>
       <c r="M22">
-        <v>16642.9</v>
+        <v>16634.89999999999</v>
       </c>
       <c r="N22">
-        <v>16899.9</v>
+        <v>16888.7</v>
       </c>
       <c r="O22">
-        <v>1015.6</v>
+        <v>1029.2</v>
       </c>
       <c r="P22">
-        <v>128.5</v>
+        <v>126.9</v>
       </c>
       <c r="Q22">
         <v>6.1</v>
       </c>
       <c r="R22">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="S22" t="s">
         <v>77</v>
@@ -3415,7 +3415,7 @@
         <v>7923421</v>
       </c>
       <c r="W22">
-        <v>12.8</v>
+        <v>13</v>
       </c>
       <c r="X22">
         <v>1.6</v>
@@ -3444,37 +3444,37 @@
         <v>4035</v>
       </c>
       <c r="G23">
-        <v>4065</v>
+        <v>4066</v>
       </c>
       <c r="H23">
-        <v>4091</v>
+        <v>4095</v>
       </c>
       <c r="I23">
-        <v>4135.999999999999</v>
+        <v>4136.199999999999</v>
       </c>
       <c r="J23">
-        <v>31.2</v>
+        <v>31.3</v>
       </c>
       <c r="K23">
         <v>1.96</v>
       </c>
       <c r="L23">
-        <v>27.3</v>
+        <v>27.4</v>
       </c>
       <c r="M23">
-        <v>4108.699999999999</v>
+        <v>4108.799999999999</v>
       </c>
       <c r="N23">
-        <v>4163.299999999999</v>
+        <v>4163.599999999999</v>
       </c>
       <c r="O23">
-        <v>-45</v>
+        <v>-41.2</v>
       </c>
       <c r="P23">
-        <v>27.3</v>
+        <v>27.4</v>
       </c>
       <c r="Q23">
-        <v>-1.1</v>
+        <v>-1</v>
       </c>
       <c r="R23">
         <v>0.6</v>
@@ -3492,10 +3492,10 @@
         <v>2427609</v>
       </c>
       <c r="W23">
-        <v>-1.9</v>
+        <v>-1.7</v>
       </c>
       <c r="X23">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="Y23" t="s">
         <v>171</v>
@@ -3678,7 +3678,7 @@
         <v>30634</v>
       </c>
       <c r="H26">
-        <v>38598</v>
+        <v>38615</v>
       </c>
       <c r="I26">
         <v>32061.00000000001</v>
@@ -3699,7 +3699,7 @@
         <v>32501.40000000001</v>
       </c>
       <c r="O26">
-        <v>6537</v>
+        <v>6554</v>
       </c>
       <c r="P26">
         <v>440.4</v>
@@ -3723,7 +3723,7 @@
         <v>8873892</v>
       </c>
       <c r="W26">
-        <v>73.7</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="X26">
         <v>4.9</v>
@@ -3909,7 +3909,7 @@
         <v>1835</v>
       </c>
       <c r="H29">
-        <v>2046</v>
+        <v>2050</v>
       </c>
       <c r="I29">
         <v>1905.400000000001</v>
@@ -3930,13 +3930,13 @@
         <v>1937.900000000001</v>
       </c>
       <c r="O29">
-        <v>140.6</v>
+        <v>144.6</v>
       </c>
       <c r="P29">
         <v>32.5</v>
       </c>
       <c r="Q29">
-        <v>7.4</v>
+        <v>7.6</v>
       </c>
       <c r="R29">
         <v>1.8</v>
@@ -3954,7 +3954,7 @@
         <v>923289</v>
       </c>
       <c r="W29">
-        <v>15.2</v>
+        <v>15.7</v>
       </c>
       <c r="X29">
         <v>3.5</v>
@@ -3986,7 +3986,7 @@
         <v>30805</v>
       </c>
       <c r="H30">
-        <v>37220</v>
+        <v>36522</v>
       </c>
       <c r="I30">
         <v>31111.80000000001</v>
@@ -4007,13 +4007,13 @@
         <v>31388.80000000001</v>
       </c>
       <c r="O30">
-        <v>6108.2</v>
+        <v>5410.2</v>
       </c>
       <c r="P30">
         <v>277</v>
       </c>
       <c r="Q30">
-        <v>19.6</v>
+        <v>17.4</v>
       </c>
       <c r="R30">
         <v>1</v>
@@ -4031,7 +4031,7 @@
         <v>21360295</v>
       </c>
       <c r="W30">
-        <v>28.6</v>
+        <v>25.3</v>
       </c>
       <c r="X30">
         <v>1.3</v>
@@ -4384,7 +4384,7 @@
         <v>16911</v>
       </c>
       <c r="H3">
-        <v>19861</v>
+        <v>19664</v>
       </c>
       <c r="I3">
         <v>17584.8</v>
@@ -4405,13 +4405,13 @@
         <v>17781.1</v>
       </c>
       <c r="O3">
-        <v>2276.2</v>
+        <v>2079.2</v>
       </c>
       <c r="P3">
         <v>196.3</v>
       </c>
       <c r="Q3">
-        <v>12.9</v>
+        <v>11.8</v>
       </c>
       <c r="R3">
         <v>1.2</v>
@@ -4429,7 +4429,7 @@
         <v>5267710</v>
       </c>
       <c r="W3">
-        <v>43.2</v>
+        <v>39.5</v>
       </c>
       <c r="X3">
         <v>3.7</v>
@@ -4461,7 +4461,7 @@
         <v>24324</v>
       </c>
       <c r="H4">
-        <v>31012</v>
+        <v>31013</v>
       </c>
       <c r="I4">
         <v>25240.6</v>
@@ -4482,7 +4482,7 @@
         <v>25584.2</v>
       </c>
       <c r="O4">
-        <v>5771.4</v>
+        <v>5772.4</v>
       </c>
       <c r="P4">
         <v>343.6</v>
@@ -4509,7 +4509,7 @@
         <v>183.6</v>
       </c>
       <c r="X4">
-        <v>10.9</v>
+        <v>11</v>
       </c>
       <c r="Y4" t="s">
         <v>277</v>
@@ -4692,7 +4692,7 @@
         <v>23948</v>
       </c>
       <c r="H7">
-        <v>27895</v>
+        <v>27901</v>
       </c>
       <c r="I7">
         <v>24747.60000000001</v>
@@ -4713,7 +4713,7 @@
         <v>25057.50000000001</v>
       </c>
       <c r="O7">
-        <v>3147.4</v>
+        <v>3153.4</v>
       </c>
       <c r="P7">
         <v>309.9</v>
@@ -4737,7 +4737,7 @@
         <v>4955221</v>
       </c>
       <c r="W7">
-        <v>63.5</v>
+        <v>63.6</v>
       </c>
       <c r="X7">
         <v>6.3</v>
@@ -4846,7 +4846,7 @@
         <v>3177</v>
       </c>
       <c r="H9">
-        <v>3505</v>
+        <v>3509</v>
       </c>
       <c r="I9">
         <v>3339.600000000001</v>
@@ -4867,13 +4867,13 @@
         <v>3414.200000000001</v>
       </c>
       <c r="O9">
-        <v>165.4</v>
+        <v>169.4</v>
       </c>
       <c r="P9">
         <v>74.59999999999999</v>
       </c>
       <c r="Q9">
-        <v>5</v>
+        <v>5.1</v>
       </c>
       <c r="R9">
         <v>2.3</v>
@@ -4891,7 +4891,7 @@
         <v>592881</v>
       </c>
       <c r="W9">
-        <v>27.9</v>
+        <v>28.6</v>
       </c>
       <c r="X9">
         <v>12.6</v>
@@ -5000,7 +5000,7 @@
         <v>99260</v>
       </c>
       <c r="H11">
-        <v>109743</v>
+        <v>109770</v>
       </c>
       <c r="I11">
         <v>101704.5999999999</v>
@@ -5021,7 +5021,7 @@
         <v>102232.7999999999</v>
       </c>
       <c r="O11">
-        <v>8038.4</v>
+        <v>8065.4</v>
       </c>
       <c r="P11">
         <v>528.2</v>
@@ -5030,7 +5030,7 @@
         <v>7.9</v>
       </c>
       <c r="R11">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="S11" t="s">
         <v>191</v>
@@ -5045,7 +5045,7 @@
         <v>30056581</v>
       </c>
       <c r="W11">
-        <v>26.7</v>
+        <v>26.8</v>
       </c>
       <c r="X11">
         <v>1.8</v>
@@ -5308,7 +5308,7 @@
         <v>76243</v>
       </c>
       <c r="H15">
-        <v>95210</v>
+        <v>95254</v>
       </c>
       <c r="I15">
         <v>80999.80000000003</v>
@@ -5329,16 +5329,16 @@
         <v>83155.10000000003</v>
       </c>
       <c r="O15">
-        <v>14210.2</v>
+        <v>14254.2</v>
       </c>
       <c r="P15">
         <v>2155.3</v>
       </c>
       <c r="Q15">
-        <v>17.5</v>
+        <v>17.6</v>
       </c>
       <c r="R15">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="S15" t="s">
         <v>195</v>
@@ -5353,7 +5353,7 @@
         <v>26213664</v>
       </c>
       <c r="W15">
-        <v>54.2</v>
+        <v>54.4</v>
       </c>
       <c r="X15">
         <v>8.199999999999999</v>
@@ -5385,7 +5385,7 @@
         <v>5943</v>
       </c>
       <c r="H16">
-        <v>6384</v>
+        <v>6534</v>
       </c>
       <c r="I16">
         <v>6562.000000000002</v>
@@ -5406,16 +5406,16 @@
         <v>6791.900000000001</v>
       </c>
       <c r="O16">
-        <v>-178</v>
+        <v>-28</v>
       </c>
       <c r="P16">
         <v>229.9</v>
       </c>
       <c r="Q16">
-        <v>-2.7</v>
+        <v>-0.4</v>
       </c>
       <c r="R16">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="S16" t="s">
         <v>196</v>
@@ -5430,7 +5430,7 @@
         <v>827822</v>
       </c>
       <c r="W16">
-        <v>-21.5</v>
+        <v>-3.4</v>
       </c>
       <c r="X16">
         <v>27.8</v>
@@ -5693,7 +5693,7 @@
         <v>657</v>
       </c>
       <c r="H20">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="I20">
         <v>653.4000000000004</v>
@@ -5714,13 +5714,13 @@
         <v>677.6000000000005</v>
       </c>
       <c r="O20">
-        <v>72.59999999999999</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="P20">
         <v>24.2</v>
       </c>
       <c r="Q20">
-        <v>11.1</v>
+        <v>11.3</v>
       </c>
       <c r="R20">
         <v>4</v>
@@ -5738,7 +5738,7 @@
         <v>249869</v>
       </c>
       <c r="W20">
-        <v>29.1</v>
+        <v>29.5</v>
       </c>
       <c r="X20">
         <v>9.6</v>
@@ -5770,7 +5770,7 @@
         <v>1515</v>
       </c>
       <c r="H21">
-        <v>1789</v>
+        <v>1762</v>
       </c>
       <c r="I21">
         <v>1471.599999999999</v>
@@ -5791,16 +5791,16 @@
         <v>1512</v>
       </c>
       <c r="O21">
-        <v>317.4</v>
+        <v>290.4</v>
       </c>
       <c r="P21">
         <v>40.4</v>
       </c>
       <c r="Q21">
-        <v>21.6</v>
+        <v>19.7</v>
       </c>
       <c r="R21">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="S21" t="s">
         <v>201</v>
@@ -5815,7 +5815,7 @@
         <v>292748</v>
       </c>
       <c r="W21">
-        <v>108.4</v>
+        <v>99.2</v>
       </c>
       <c r="X21">
         <v>13.8</v>
@@ -5835,49 +5835,49 @@
         <v>23635</v>
       </c>
       <c r="D22">
-        <v>23099</v>
+        <v>23056</v>
       </c>
       <c r="E22">
-        <v>22999</v>
+        <v>22968</v>
       </c>
       <c r="F22">
-        <v>23243</v>
+        <v>23206</v>
       </c>
       <c r="G22">
-        <v>22896</v>
+        <v>22859</v>
       </c>
       <c r="H22">
-        <v>25800</v>
+        <v>25841</v>
       </c>
       <c r="I22">
-        <v>23607.2</v>
+        <v>23577.59999999999</v>
       </c>
       <c r="J22">
-        <v>257.2</v>
+        <v>270.1</v>
       </c>
       <c r="K22">
         <v>1.96</v>
       </c>
       <c r="L22">
-        <v>225.4</v>
+        <v>236.8</v>
       </c>
       <c r="M22">
-        <v>23381.8</v>
+        <v>23340.8</v>
       </c>
       <c r="N22">
-        <v>23832.6</v>
+        <v>23814.39999999999</v>
       </c>
       <c r="O22">
-        <v>2192.8</v>
+        <v>2263.4</v>
       </c>
       <c r="P22">
-        <v>225.4</v>
+        <v>236.8</v>
       </c>
       <c r="Q22">
-        <v>9.300000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="S22" t="s">
         <v>202</v>
@@ -5892,10 +5892,10 @@
         <v>8028876</v>
       </c>
       <c r="W22">
-        <v>27.3</v>
+        <v>28.2</v>
       </c>
       <c r="X22">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="Y22" t="s">
         <v>295</v>
@@ -5918,37 +5918,37 @@
         <v>6132</v>
       </c>
       <c r="F23">
-        <v>6133</v>
+        <v>6134</v>
       </c>
       <c r="G23">
-        <v>6140</v>
+        <v>6142</v>
       </c>
       <c r="H23">
-        <v>6217</v>
+        <v>6218</v>
       </c>
       <c r="I23">
-        <v>6324.4</v>
+        <v>6325</v>
       </c>
       <c r="J23">
-        <v>68.8</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="K23">
         <v>1.96</v>
       </c>
       <c r="L23">
-        <v>60.3</v>
+        <v>60</v>
       </c>
       <c r="M23">
-        <v>6264.099999999999</v>
+        <v>6265</v>
       </c>
       <c r="N23">
-        <v>6384.7</v>
+        <v>6385</v>
       </c>
       <c r="O23">
-        <v>-107.4</v>
+        <v>-107</v>
       </c>
       <c r="P23">
-        <v>60.3</v>
+        <v>60</v>
       </c>
       <c r="Q23">
         <v>-1.7</v>
@@ -6155,7 +6155,7 @@
         <v>61732</v>
       </c>
       <c r="H26">
-        <v>75826</v>
+        <v>75864</v>
       </c>
       <c r="I26">
         <v>62731.00000000002</v>
@@ -6176,7 +6176,7 @@
         <v>63459.70000000002</v>
       </c>
       <c r="O26">
-        <v>13095</v>
+        <v>13133</v>
       </c>
       <c r="P26">
         <v>728.7</v>
@@ -6200,7 +6200,7 @@
         <v>8889343</v>
       </c>
       <c r="W26">
-        <v>147.3</v>
+        <v>147.7</v>
       </c>
       <c r="X26">
         <v>8.199999999999999</v>
@@ -6309,7 +6309,7 @@
         <v>13540</v>
       </c>
       <c r="H28">
-        <v>15288</v>
+        <v>15290</v>
       </c>
       <c r="I28">
         <v>13804.2</v>
@@ -6330,16 +6330,16 @@
         <v>13966.8</v>
       </c>
       <c r="O28">
-        <v>1483.8</v>
+        <v>1485.8</v>
       </c>
       <c r="P28">
         <v>162.6</v>
       </c>
       <c r="Q28">
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
       <c r="R28">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="S28" t="s">
         <v>208</v>
@@ -6354,7 +6354,7 @@
         <v>2549303</v>
       </c>
       <c r="W28">
-        <v>58.2</v>
+        <v>58.3</v>
       </c>
       <c r="X28">
         <v>6.4</v>
@@ -6386,7 +6386,7 @@
         <v>3697</v>
       </c>
       <c r="H29">
-        <v>4220</v>
+        <v>4235</v>
       </c>
       <c r="I29">
         <v>3824.2</v>
@@ -6407,13 +6407,13 @@
         <v>3902.8</v>
       </c>
       <c r="O29">
-        <v>395.8</v>
+        <v>410.8</v>
       </c>
       <c r="P29">
         <v>78.59999999999999</v>
       </c>
       <c r="Q29">
-        <v>10.3</v>
+        <v>10.7</v>
       </c>
       <c r="R29">
         <v>2.2</v>
@@ -6431,7 +6431,7 @@
         <v>979172</v>
       </c>
       <c r="W29">
-        <v>40.4</v>
+        <v>42</v>
       </c>
       <c r="X29">
         <v>8</v>
@@ -6463,7 +6463,7 @@
         <v>61265</v>
       </c>
       <c r="H30">
-        <v>73174</v>
+        <v>72694</v>
       </c>
       <c r="I30">
         <v>62990.99999999999</v>
@@ -6484,13 +6484,13 @@
         <v>63420.99999999999</v>
       </c>
       <c r="O30">
-        <v>10183</v>
+        <v>9703</v>
       </c>
       <c r="P30">
         <v>430</v>
       </c>
       <c r="Q30">
-        <v>16.2</v>
+        <v>15.4</v>
       </c>
       <c r="R30">
         <v>0.8</v>
@@ -6508,7 +6508,7 @@
         <v>21361086</v>
       </c>
       <c r="W30">
-        <v>47.7</v>
+        <v>45.4</v>
       </c>
       <c r="X30">
         <v>2</v>
@@ -6861,7 +6861,7 @@
         <v>27511</v>
       </c>
       <c r="H3">
-        <v>31633</v>
+        <v>31385</v>
       </c>
       <c r="I3">
         <v>28307.79999999999</v>
@@ -6882,13 +6882,13 @@
         <v>28542.29999999999</v>
       </c>
       <c r="O3">
-        <v>3325.2</v>
+        <v>3077.2</v>
       </c>
       <c r="P3">
         <v>234.5</v>
       </c>
       <c r="Q3">
-        <v>11.7</v>
+        <v>10.9</v>
       </c>
       <c r="R3">
         <v>0.9</v>
@@ -6906,10 +6906,10 @@
         <v>10488373</v>
       </c>
       <c r="W3">
-        <v>31.7</v>
+        <v>29.3</v>
       </c>
       <c r="X3">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="Y3" t="s">
         <v>401</v>
@@ -6938,7 +6938,7 @@
         <v>37281</v>
       </c>
       <c r="H4">
-        <v>47915</v>
+        <v>47920</v>
       </c>
       <c r="I4">
         <v>38786.00000000001</v>
@@ -6959,7 +6959,7 @@
         <v>39286.70000000001</v>
       </c>
       <c r="O4">
-        <v>9129</v>
+        <v>9134</v>
       </c>
       <c r="P4">
         <v>500.7</v>
@@ -6983,7 +6983,7 @@
         <v>6329301</v>
       </c>
       <c r="W4">
-        <v>144.2</v>
+        <v>144.3</v>
       </c>
       <c r="X4">
         <v>7.9</v>
@@ -7169,7 +7169,7 @@
         <v>36850</v>
       </c>
       <c r="H7">
-        <v>42719</v>
+        <v>42724</v>
       </c>
       <c r="I7">
         <v>38151.60000000001</v>
@@ -7190,7 +7190,7 @@
         <v>38641.7</v>
       </c>
       <c r="O7">
-        <v>4567.4</v>
+        <v>4572.4</v>
       </c>
       <c r="P7">
         <v>490.1</v>
@@ -7323,7 +7323,7 @@
         <v>4684</v>
       </c>
       <c r="H9">
-        <v>5250</v>
+        <v>5256</v>
       </c>
       <c r="I9">
         <v>4937.799999999997</v>
@@ -7344,13 +7344,13 @@
         <v>5054.899999999998</v>
       </c>
       <c r="O9">
-        <v>312.2</v>
+        <v>318.2</v>
       </c>
       <c r="P9">
         <v>117.1</v>
       </c>
       <c r="Q9">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="R9">
         <v>2.4</v>
@@ -7368,7 +7368,7 @@
         <v>1202898</v>
       </c>
       <c r="W9">
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="X9">
         <v>9.699999999999999</v>
@@ -7477,7 +7477,7 @@
         <v>152705</v>
       </c>
       <c r="H11">
-        <v>168068</v>
+        <v>168102</v>
       </c>
       <c r="I11">
         <v>155221.6</v>
@@ -7498,7 +7498,7 @@
         <v>155841</v>
       </c>
       <c r="O11">
-        <v>12846.4</v>
+        <v>12880.4</v>
       </c>
       <c r="P11">
         <v>619.4</v>
@@ -7507,7 +7507,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S11" t="s">
         <v>316</v>
@@ -7785,7 +7785,7 @@
         <v>122913</v>
       </c>
       <c r="H15">
-        <v>149592</v>
+        <v>149647</v>
       </c>
       <c r="I15">
         <v>129963.7999999999</v>
@@ -7806,7 +7806,7 @@
         <v>133179.5999999999</v>
       </c>
       <c r="O15">
-        <v>19628.2</v>
+        <v>19683.2</v>
       </c>
       <c r="P15">
         <v>3215.8</v>
@@ -7815,7 +7815,7 @@
         <v>15.1</v>
       </c>
       <c r="R15">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="S15" t="s">
         <v>320</v>
@@ -7830,10 +7830,10 @@
         <v>52577772</v>
       </c>
       <c r="W15">
-        <v>37.3</v>
+        <v>37.4</v>
       </c>
       <c r="X15">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="Y15" t="s">
         <v>413</v>
@@ -7862,7 +7862,7 @@
         <v>9086</v>
       </c>
       <c r="H16">
-        <v>9711</v>
+        <v>9895</v>
       </c>
       <c r="I16">
         <v>10008.8</v>
@@ -7883,16 +7883,16 @@
         <v>10365.4</v>
       </c>
       <c r="O16">
-        <v>-297.8</v>
+        <v>-113.8</v>
       </c>
       <c r="P16">
         <v>356.6</v>
       </c>
       <c r="Q16">
-        <v>-3</v>
+        <v>-1.1</v>
       </c>
       <c r="R16">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="S16" t="s">
         <v>321</v>
@@ -7907,7 +7907,7 @@
         <v>1716436</v>
       </c>
       <c r="W16">
-        <v>-17.3</v>
+        <v>-6.6</v>
       </c>
       <c r="X16">
         <v>20.7</v>
@@ -8170,7 +8170,7 @@
         <v>1044</v>
       </c>
       <c r="H20">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="I20">
         <v>1057.6</v>
@@ -8191,13 +8191,13 @@
         <v>1090.6</v>
       </c>
       <c r="O20">
-        <v>86.40000000000001</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="P20">
         <v>33</v>
       </c>
       <c r="Q20">
-        <v>8.199999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="R20">
         <v>3.3</v>
@@ -8215,10 +8215,10 @@
         <v>476286</v>
       </c>
       <c r="W20">
-        <v>18.1</v>
+        <v>18.8</v>
       </c>
       <c r="X20">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="Y20" t="s">
         <v>418</v>
@@ -8247,7 +8247,7 @@
         <v>2328</v>
       </c>
       <c r="H21">
-        <v>2799</v>
+        <v>2762</v>
       </c>
       <c r="I21">
         <v>2335.6</v>
@@ -8268,13 +8268,13 @@
         <v>2383.5</v>
       </c>
       <c r="O21">
-        <v>463.4</v>
+        <v>426.4</v>
       </c>
       <c r="P21">
         <v>47.9</v>
       </c>
       <c r="Q21">
-        <v>19.8</v>
+        <v>18.3</v>
       </c>
       <c r="R21">
         <v>2.4</v>
@@ -8292,7 +8292,7 @@
         <v>584830</v>
       </c>
       <c r="W21">
-        <v>79.2</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="X21">
         <v>8.199999999999999</v>
@@ -8309,52 +8309,52 @@
         <v>46</v>
       </c>
       <c r="C22">
-        <v>40248</v>
+        <v>40249</v>
       </c>
       <c r="D22">
-        <v>39594</v>
+        <v>39526</v>
       </c>
       <c r="E22">
-        <v>39180</v>
+        <v>39146</v>
       </c>
       <c r="F22">
-        <v>39773</v>
+        <v>39717</v>
       </c>
       <c r="G22">
-        <v>39338</v>
+        <v>39299</v>
       </c>
       <c r="H22">
-        <v>43587</v>
+        <v>43632</v>
       </c>
       <c r="I22">
-        <v>40378.60000000001</v>
+        <v>40339.39999999999</v>
       </c>
       <c r="J22">
-        <v>371.9</v>
+        <v>383.7</v>
       </c>
       <c r="K22">
         <v>1.96</v>
       </c>
       <c r="L22">
-        <v>326</v>
+        <v>336.3</v>
       </c>
       <c r="M22">
-        <v>40052.60000000001</v>
+        <v>40003.09999999999</v>
       </c>
       <c r="N22">
-        <v>40704.60000000001</v>
+        <v>40675.7</v>
       </c>
       <c r="O22">
-        <v>3208.4</v>
+        <v>3292.6</v>
       </c>
       <c r="P22">
-        <v>326</v>
+        <v>336.3</v>
       </c>
       <c r="Q22">
-        <v>7.9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="R22">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="S22" t="s">
         <v>327</v>
@@ -8369,7 +8369,7 @@
         <v>15952297</v>
       </c>
       <c r="W22">
-        <v>20.1</v>
+        <v>20.6</v>
       </c>
       <c r="X22">
         <v>2.1</v>
@@ -8395,40 +8395,40 @@
         <v>10254</v>
       </c>
       <c r="F23">
-        <v>10168</v>
+        <v>10169</v>
       </c>
       <c r="G23">
-        <v>10205</v>
+        <v>10208</v>
       </c>
       <c r="H23">
-        <v>10308</v>
+        <v>10313</v>
       </c>
       <c r="I23">
-        <v>10460.40000000001</v>
+        <v>10461.20000000001</v>
       </c>
       <c r="J23">
-        <v>64.2</v>
+        <v>63.5</v>
       </c>
       <c r="K23">
         <v>1.96</v>
       </c>
       <c r="L23">
-        <v>56.3</v>
+        <v>55.7</v>
       </c>
       <c r="M23">
-        <v>10404.10000000001</v>
+        <v>10405.50000000001</v>
       </c>
       <c r="N23">
-        <v>10516.70000000001</v>
+        <v>10516.90000000001</v>
       </c>
       <c r="O23">
-        <v>-152.4</v>
+        <v>-148.2</v>
       </c>
       <c r="P23">
-        <v>56.3</v>
+        <v>55.7</v>
       </c>
       <c r="Q23">
-        <v>-1.5</v>
+        <v>-1.4</v>
       </c>
       <c r="R23">
         <v>0.5</v>
@@ -8446,10 +8446,10 @@
         <v>4960488</v>
       </c>
       <c r="W23">
-        <v>-3.1</v>
+        <v>-3</v>
       </c>
       <c r="X23">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="Y23" t="s">
         <v>421</v>
@@ -8632,7 +8632,7 @@
         <v>92366</v>
       </c>
       <c r="H26">
-        <v>114424</v>
+        <v>114479</v>
       </c>
       <c r="I26">
         <v>94792</v>
@@ -8653,13 +8653,13 @@
         <v>95729.5</v>
       </c>
       <c r="O26">
-        <v>19632</v>
+        <v>19687</v>
       </c>
       <c r="P26">
         <v>937.5</v>
       </c>
       <c r="Q26">
-        <v>20.7</v>
+        <v>20.8</v>
       </c>
       <c r="R26">
         <v>1.2</v>
@@ -8677,7 +8677,7 @@
         <v>17763235</v>
       </c>
       <c r="W26">
-        <v>110.5</v>
+        <v>110.8</v>
       </c>
       <c r="X26">
         <v>5.3</v>
@@ -8786,7 +8786,7 @@
         <v>20416</v>
       </c>
       <c r="H28">
-        <v>23309</v>
+        <v>23311</v>
       </c>
       <c r="I28">
         <v>20947.8</v>
@@ -8807,7 +8807,7 @@
         <v>21169.3</v>
       </c>
       <c r="O28">
-        <v>2361.2</v>
+        <v>2363.2</v>
       </c>
       <c r="P28">
         <v>221.5</v>
@@ -8863,7 +8863,7 @@
         <v>5532</v>
       </c>
       <c r="H29">
-        <v>6266</v>
+        <v>6285</v>
       </c>
       <c r="I29">
         <v>5729.600000000004</v>
@@ -8884,13 +8884,13 @@
         <v>5834.600000000004</v>
       </c>
       <c r="O29">
-        <v>536.4</v>
+        <v>555.4</v>
       </c>
       <c r="P29">
         <v>105</v>
       </c>
       <c r="Q29">
-        <v>9.4</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="R29">
         <v>2</v>
@@ -8908,7 +8908,7 @@
         <v>1902461</v>
       </c>
       <c r="W29">
-        <v>28.2</v>
+        <v>29.2</v>
       </c>
       <c r="X29">
         <v>5.5</v>
@@ -8940,7 +8940,7 @@
         <v>92070</v>
       </c>
       <c r="H30">
-        <v>110418</v>
+        <v>109216</v>
       </c>
       <c r="I30">
         <v>94102.79999999997</v>
@@ -8961,16 +8961,16 @@
         <v>94541.89999999998</v>
       </c>
       <c r="O30">
-        <v>16315.2</v>
+        <v>15113.2</v>
       </c>
       <c r="P30">
         <v>439.1</v>
       </c>
       <c r="Q30">
-        <v>17.3</v>
+        <v>16.1</v>
       </c>
       <c r="R30">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="S30" t="s">
         <v>335</v>
@@ -8985,7 +8985,7 @@
         <v>42721381</v>
       </c>
       <c r="W30">
-        <v>38.2</v>
+        <v>35.4</v>
       </c>
       <c r="X30">
         <v>1</v>

</xml_diff>